<commit_message>
Deploying to gh-pages from @ ScienceBasedTargets/SBTi-finance-tool@f8b8f07eb5463a9117ddeac3ee586a660c708e8f 🚀
</commit_message>
<xml_diff>
--- a/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
+++ b/_downloads/d16600f8589c0c47112a7407bd6f0c23/DataProviderTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mountainrambler\SBTi\SBTi-finance-tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_BCCFA2BD0AFE4771E24C6D0DBC87A6ED4B30D22F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35A3BBCA-F2EF-46A8-B156-4D9ACA454480}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3473014C-3352-4A89-AE1D-59AB3636BE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32025" yWindow="3225" windowWidth="38700" windowHeight="15285" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>company_name</t>
   </si>
@@ -199,13 +199,25 @@
   </si>
   <si>
     <t>Steel</t>
+  </si>
+  <si>
+    <t>target_ids</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,9 +312,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:P120" totalsRowShown="0">
-  <autoFilter ref="A1:P120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:Q120" totalsRowShown="0">
+  <autoFilter ref="A1:Q120" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
@@ -319,6 +331,7 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="base_year_ghg_s2"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="base_year_ghg_s3"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="achieved_reduction"/>
+    <tableColumn id="17" xr3:uid="{5F0CB71F-8752-4977-A490-27DCA30723FC}" name="target_ids"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -593,20 +606,20 @@
       <selection activeCell="K2" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="21.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="21.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -712,7 +725,7 @@
         <v>990719858</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -778,25 +791,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="4" width="21.109375" customWidth="1"/>
+    <col min="6" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,8 +858,11 @@
       <c r="P1" t="s">
         <v>48</v>
       </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -886,8 +902,11 @@
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="Q2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -930,9 +949,11 @@
       <c r="P3">
         <v>0.1</v>
       </c>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -977,6 +998,9 @@
       </c>
       <c r="P4">
         <v>0.1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -989,6 +1013,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -1160,29 +1199,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEEFA7D1-1829-4AA1-B93C-54856ECD839E}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3819C-57C4-4F13-9AF5-6CCD1D9AA3D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6280943-A9F4-43BE-9F92-E31CF54894DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>